<commit_message>
15 , 16 17
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t xml:space="preserve">Externo</t>
   </si>
@@ -61,121 +61,103 @@
     <t xml:space="preserve">FB</t>
   </si>
   <si>
-    <t xml:space="preserve">Comercial envia solicitação de produção</t>
+    <t xml:space="preserve">Responsável pelo comercial envia solicitação de produção</t>
   </si>
   <si>
     <t xml:space="preserve">x</t>
   </si>
   <si>
-    <t xml:space="preserve">Gerência analisa solicitação de produção</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(1)x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerência emite ordem de produção</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2)x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Produzir Subcomponentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerencia envia ordem de produção</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(3)x</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linha de produção separa componente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4(x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linha de produção fixa componente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5(x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linha de produção solda componentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6(x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linha de produção verificar ordem de produção</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7(x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linha de produção realiza re-trabalho</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Testar subcomponentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linha de produção envia subcomponente não testado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8(x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Controle de qualidade testa subcomponente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">9(x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Montar a maquina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Controle de qualidade fixa subcomponentes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11(x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Controle de qualidade empacota máquina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12(x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Controle de qualidade encaminha máquina montada</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13(x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Entregar maquina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Controle de qualidade envia máquina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14(x)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerência despacha maquina</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15(x)</t>
+    <t xml:space="preserve">Gerente de produção analisa solicitação de produção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Produzir subcomponente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerente de produção envia ordem de produção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operário separa componentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(3)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operário fixa componentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(4)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operário solda componentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(5)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operário realiza retrabalho</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Montar máquina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Operário envia subcomponente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Técnico testa subcomponente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(8)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Técnico fixa sub componente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(9)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Técnico embala máquina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entregar máquina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Técnico envia máquina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(11)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerente de produção encaminha máquina</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(12)</t>
   </si>
   <si>
     <t xml:space="preserve">Priorizar pedido</t>
   </si>
   <si>
-    <t xml:space="preserve">Negócios envia pedido de prioridade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gerência prioriza pedido</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(x)17</t>
+    <t xml:space="preserve">Gerente de negócios envia pedido priorizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gerente de produção envia ordem de produção priorizada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X(14)</t>
   </si>
 </sst>
 </file>
@@ -186,7 +168,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -217,6 +199,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="10.5"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="7.5"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -245,6 +234,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
       <sz val="10.5"/>
       <color rgb="FF111111"/>
       <name val="Arial"/>
@@ -259,13 +254,24 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -298,32 +304,26 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF34A852"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4285F4"/>
-        <bgColor rgb="FF666699"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF4000"/>
         <bgColor rgb="FFFF0000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF55308D"/>
-        <bgColor rgb="FF333333"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFBF0041"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFFF4000"/>
+        <fgColor rgb="FFBF0041"/>
+        <bgColor rgb="FF800080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2A6099"/>
+        <bgColor rgb="FF666699"/>
       </patternFill>
     </fill>
   </fills>
@@ -393,19 +393,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -413,7 +413,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -425,14 +425,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -441,11 +433,19 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -453,11 +453,19 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -465,24 +473,16 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -512,7 +512,7 @@
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
-      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FFBF0041"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
@@ -522,7 +522,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF2A6099"/>
       <rgbColor rgb="FFCFE1F2"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -540,7 +540,7 @@
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFF4CCCC"/>
-      <rgbColor rgb="FF4285F4"/>
+      <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFBBC04"/>
@@ -549,12 +549,12 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF34A852"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF111111"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF55308D"/>
+      <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
@@ -566,13 +566,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.65234375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.33"/>
@@ -580,9 +580,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="60.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="33.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="14.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -654,8 +654,12 @@
       <c r="J3" s="13"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
+      <c r="A4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" s="8" t="n">
         <v>2</v>
       </c>
@@ -672,27 +676,29 @@
       <c r="J4" s="13"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C5" s="8" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="10"/>
+        <v>18</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>19</v>
+      </c>
       <c r="F5" s="10"/>
-      <c r="G5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
       <c r="I5" s="12"/>
       <c r="J5" s="13"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="s">
-        <v>19</v>
-      </c>
+      <c r="A6" s="16"/>
       <c r="B6" s="7" t="s">
         <v>12</v>
       </c>
@@ -702,44 +708,44 @@
       <c r="D6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="21" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="22"/>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C8" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="10"/>
@@ -752,7 +758,7 @@
       <c r="J8" s="13"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
@@ -772,7 +778,9 @@
       <c r="J9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18"/>
+      <c r="A10" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
@@ -780,40 +788,42 @@
         <v>8</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="10"/>
+        <v>29</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="F10" s="10"/>
-      <c r="G10" s="14" t="s">
-        <v>29</v>
-      </c>
+      <c r="G10" s="14"/>
       <c r="H10" s="15"/>
       <c r="I10" s="12"/>
       <c r="J10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18"/>
+      <c r="A11" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="B11" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="D11" s="22" t="s">
-        <v>30</v>
+      <c r="D11" s="24" t="s">
+        <v>31</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="23" t="s">
-        <v>29</v>
+      <c r="G11" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="s">
-        <v>31</v>
+      <c r="A12" s="23" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>12</v>
@@ -821,41 +831,43 @@
       <c r="C12" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="D12" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="19" t="s">
+      <c r="D12" s="26" t="s">
         <v>33</v>
       </c>
+      <c r="E12" s="19"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="12"/>
+      <c r="G12" s="12" t="s">
+        <v>34</v>
+      </c>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24"/>
+      <c r="A13" s="23" t="s">
+        <v>28</v>
+      </c>
       <c r="B13" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>34</v>
+      <c r="D13" s="26" t="s">
+        <v>35</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H13" s="21"/>
+      <c r="G13" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="22"/>
       <c r="I13" s="12"/>
       <c r="J13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26" t="s">
-        <v>36</v>
+      <c r="A14" s="27" t="s">
+        <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>12</v>
@@ -863,43 +875,39 @@
       <c r="C14" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="D14" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="D14" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>39</v>
+      </c>
       <c r="F14" s="10"/>
-      <c r="G14" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="H14" s="21"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
       <c r="I14" s="12"/>
       <c r="J14" s="13"/>
     </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="26" t="s">
-        <v>36</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>12</v>
-      </c>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="27"/>
+      <c r="B15" s="7"/>
       <c r="C15" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="D15" s="25" t="s">
-        <v>39</v>
+      <c r="D15" s="26" t="s">
+        <v>40</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" s="21"/>
+      <c r="G15" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="12"/>
       <c r="I15" s="12"/>
       <c r="J15" s="13"/>
     </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26" t="s">
-        <v>36</v>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="28" t="s">
+        <v>42</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>12</v>
@@ -907,121 +915,55 @@
       <c r="C16" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="D16" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="21" t="s">
-        <v>42</v>
-      </c>
+      <c r="D16" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="19"/>
+      <c r="F16" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="12"/>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
       <c r="J16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>12</v>
-      </c>
+      <c r="A17" s="28"/>
+      <c r="B17" s="7"/>
       <c r="C17" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="F17" s="10"/>
-      <c r="G17" s="12"/>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="13"/>
     </row>
-    <row r="18" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="8" t="n">
-        <v>16</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="13"/>
-    </row>
+    <row r="18" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="8" t="n">
-        <v>17</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="E19" s="10"/>
-      <c r="F19" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="13"/>
-    </row>
-    <row r="20" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="28"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8" t="n">
-        <v>18</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="13"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D22" s="29"/>
-    </row>
+      <c r="D19" s="29"/>
+    </row>
+    <row r="20" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="12">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="A6:A11"/>
-    <mergeCell ref="B6:B11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
amanha  e o dia
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -168,7 +168,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -238,6 +238,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -254,15 +255,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
@@ -368,7 +365,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,19 +450,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -477,11 +470,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -569,10 +562,10 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J18" activeCellId="0" sqref="J18"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.61328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.33"/>
@@ -725,15 +718,15 @@
       <c r="C7" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="9" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="20"/>
       <c r="F7" s="10"/>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="22"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
     </row>
@@ -745,7 +738,7 @@
       <c r="C8" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="9" t="s">
         <v>24</v>
       </c>
       <c r="E8" s="10"/>
@@ -778,7 +771,7 @@
       <c r="J9" s="13"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="7" t="s">
@@ -800,7 +793,7 @@
       <c r="J10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -809,12 +802,12 @@
       <c r="C11" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="23" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="25" t="s">
+      <c r="G11" s="24" t="s">
         <v>32</v>
       </c>
       <c r="H11" s="12"/>
@@ -822,7 +815,7 @@
       <c r="J11" s="13"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -831,7 +824,7 @@
       <c r="C12" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="D12" s="26" t="s">
+      <c r="D12" s="25" t="s">
         <v>33</v>
       </c>
       <c r="E12" s="19"/>
@@ -844,7 +837,7 @@
       <c r="J12" s="13"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="7" t="s">
@@ -853,20 +846,20 @@
       <c r="C13" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="25" t="s">
         <v>35</v>
       </c>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="22"/>
+      <c r="H13" s="21"/>
       <c r="I13" s="12"/>
       <c r="J13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="26" t="s">
         <v>37</v>
       </c>
       <c r="B14" s="7" t="s">
@@ -875,30 +868,30 @@
       <c r="C14" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="D14" s="26" t="s">
+      <c r="D14" s="25" t="s">
         <v>38</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>39</v>
       </c>
       <c r="F14" s="10"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
       <c r="I14" s="12"/>
       <c r="J14" s="13"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="25" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="10"/>
       <c r="F15" s="10"/>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="21" t="s">
         <v>41</v>
       </c>
       <c r="H15" s="12"/>
@@ -906,7 +899,7 @@
       <c r="J15" s="13"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="28" t="s">
+      <c r="A16" s="27" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -915,7 +908,7 @@
       <c r="C16" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="D16" s="26" t="s">
+      <c r="D16" s="25" t="s">
         <v>43</v>
       </c>
       <c r="E16" s="19"/>
@@ -928,17 +921,17 @@
       <c r="J16" s="13"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28"/>
+      <c r="A17" s="27"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="D17" s="26" t="s">
+      <c r="D17" s="25" t="s">
         <v>44</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="21" t="s">
         <v>45</v>
       </c>
       <c r="H17" s="12"/>
@@ -947,7 +940,7 @@
     </row>
     <row r="18" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D19" s="29"/>
+      <c r="D19" s="28"/>
     </row>
     <row r="20" customFormat="false" ht="30.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>

<commit_message>
Artefato 19 comitado e corrigido para pdf
</commit_message>
<xml_diff>
--- a/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
+++ b/Artefatos/17. Análise dos Eventos para cada Cenário.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -561,11 +561,11 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.33"/>

</xml_diff>